<commit_message>
[quiz] [QUEST-2] README enrichment #time 0d 8h 0m
</commit_message>
<xml_diff>
--- a/static/questions.xlsx
+++ b/static/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\Documents\Code\quiz\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1F1113-4BC7-46F4-AA70-442CF42D19B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BC36A2-3052-4989-9179-018C284F0B40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="-14430" windowWidth="14400" windowHeight="7365" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quiz" sheetId="1" r:id="rId1"/>
@@ -474,12 +474,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,6 +505,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,562 +901,559 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.453125" customWidth="1"/>
-    <col min="5" max="5" width="37" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.90625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47.36328125" customWidth="1"/>
+    <col min="5" max="8" width="26.26953125" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.7265625" customWidth="1"/>
     <col min="10" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>100</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>500</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>5050</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>1001</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>1050</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>10010</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>7.5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>3.75</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>488</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>271</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>512</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>13</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>15</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>20</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>67</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>66</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>68</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>1</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>1</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>1</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>3</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>98</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>5</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="8">
+        <v>400</v>
+      </c>
+      <c r="F20" s="7">
+        <v>750</v>
+      </c>
+      <c r="G20" s="7">
         <v>800</v>
       </c>
-      <c r="F20" s="8">
-        <v>750</v>
-      </c>
-      <c r="G20" s="9">
-        <v>400</v>
-      </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>1</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>